<commit_message>
Mise à jour XL
</commit_message>
<xml_diff>
--- a/TableurBoursiere.xlsx
+++ b/TableurBoursiere.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\majer\OneDrive\Documents\Paul\ProgrammesR\boursiR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0064BB22-A25F-4BB4-915F-E45EEC39842D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F09F6615-802E-4290-86E8-72E1E9B009D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F1ED27E7-026F-451E-903D-1295AC011CBD}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="50">
   <si>
     <t>Bière</t>
   </si>
@@ -185,6 +185,9 @@
   </si>
   <si>
     <t>Prix suggéré programme R</t>
+  </si>
+  <si>
+    <t>Augmentation R</t>
   </si>
 </sst>
 </file>
@@ -628,7 +631,7 @@
   <dimension ref="A1:V74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -639,9 +642,9 @@
     <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.42578125" customWidth="1"/>
+    <col min="8" max="8" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.42578125" customWidth="1"/>
     <col min="12" max="12" width="14.85546875" customWidth="1"/>
     <col min="13" max="13" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="11.28515625" bestFit="1" customWidth="1"/>
@@ -673,12 +676,14 @@
       <c r="H1" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="I1" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="J1" s="13"/>
-      <c r="K1" s="11" t="s">
-        <v>8</v>
+      <c r="K1" s="13" t="s">
+        <v>49</v>
       </c>
       <c r="L1" s="11" t="s">
         <v>22</v>
@@ -740,29 +745,29 @@
         <v>2.5</v>
       </c>
       <c r="H2" s="9">
-        <f t="shared" ref="H2:H19" si="0">G2+T2</f>
+        <f>G2+T2</f>
         <v>5.8</v>
       </c>
-      <c r="I2" s="9">
+      <c r="I2" s="1">
+        <f>H2-G2</f>
+        <v>3.3</v>
+      </c>
+      <c r="J2" s="9">
         <v>3.67</v>
       </c>
-      <c r="J2" s="1">
-        <f>I2-G2</f>
+      <c r="K2" s="1">
+        <f>J2-G2</f>
         <v>1.17</v>
       </c>
-      <c r="K2" s="1">
-        <f t="shared" ref="K2:K19" si="1">H2-G2</f>
-        <v>3.3</v>
-      </c>
       <c r="L2" s="4">
-        <f t="shared" ref="L2:L19" si="2">K2/G2</f>
+        <f>I2/G2</f>
         <v>1.3199999999999998</v>
       </c>
       <c r="M2" s="8">
         <v>35</v>
       </c>
       <c r="N2" s="5">
-        <f t="shared" ref="N2:N19" si="3">M2/SUM($M$2:$M$16)</f>
+        <f t="shared" ref="N2:N19" si="0">M2/SUM($M$2:$M$16)</f>
         <v>0.16431924882629109</v>
       </c>
       <c r="O2" s="3">
@@ -778,11 +783,11 @@
         <v>1.7147887323943662</v>
       </c>
       <c r="R2" s="1">
-        <f t="shared" ref="R2:R19" si="4">G2-E2</f>
+        <f>G2-E2</f>
         <v>0.89999999999999991</v>
       </c>
       <c r="S2" s="1">
-        <f t="shared" ref="S2:S19" si="5">F2-D2</f>
+        <f>F2-D2</f>
         <v>1.9000000000000004</v>
       </c>
       <c r="T2" s="2">
@@ -811,7 +816,7 @@
         <v>2.5</v>
       </c>
       <c r="E3" s="10">
-        <f t="shared" ref="E3:E19" si="6">ROUND(0.5+C3,1)</f>
+        <f t="shared" ref="E3:E19" si="1">ROUND(0.5+C3,1)</f>
         <v>1.4</v>
       </c>
       <c r="F3" s="10">
@@ -819,57 +824,57 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="G3" s="1">
-        <f t="shared" ref="G3:G19" si="7">D3</f>
+        <f t="shared" ref="G3:G19" si="2">D3</f>
         <v>2.5</v>
       </c>
       <c r="H3" s="9">
-        <f t="shared" si="0"/>
+        <f>G3+T3</f>
         <v>4.5</v>
       </c>
-      <c r="I3" s="9">
+      <c r="I3" s="1">
+        <f>H3-G3</f>
+        <v>2</v>
+      </c>
+      <c r="J3" s="9">
         <v>2.5</v>
       </c>
-      <c r="J3" s="1">
-        <f t="shared" ref="J3:J19" si="8">I3-G3</f>
-        <v>0</v>
-      </c>
       <c r="K3" s="1">
-        <f t="shared" si="1"/>
-        <v>2</v>
+        <f>J3-G3</f>
+        <v>0</v>
       </c>
       <c r="L3" s="4">
-        <f t="shared" si="2"/>
+        <f>I3/G3</f>
         <v>0.8</v>
       </c>
       <c r="M3" s="8">
         <v>24</v>
       </c>
       <c r="N3" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>0.11267605633802817</v>
       </c>
       <c r="O3" s="3">
-        <f t="shared" ref="O3:O19" si="9">1/20</f>
+        <f t="shared" ref="O3:O19" si="3">1/20</f>
         <v>0.05</v>
       </c>
       <c r="P3" s="6">
-        <f t="shared" ref="P3:P12" si="10">N3-O3</f>
+        <f t="shared" ref="P3:P12" si="4">N3-O3</f>
         <v>6.2676056338028169E-2</v>
       </c>
       <c r="Q3" s="3">
-        <f t="shared" ref="Q3:Q12" si="11">P3*$U$2</f>
+        <f t="shared" ref="Q3:Q12" si="5">P3*$U$2</f>
         <v>0.9401408450704225</v>
       </c>
       <c r="R3" s="1">
-        <f t="shared" si="4"/>
+        <f>G3-E3</f>
         <v>1.1000000000000001</v>
       </c>
       <c r="S3" s="1">
-        <f t="shared" si="5"/>
+        <f>F3-D3</f>
         <v>2.0999999999999996</v>
       </c>
       <c r="T3" s="2">
-        <f t="shared" ref="T3:T12" si="12">ROUND(IF(P3&gt;0,S3*Q3,R3*Q3),1)</f>
+        <f t="shared" ref="T3:T12" si="6">ROUND(IF(P3&gt;0,S3*Q3,R3*Q3),1)</f>
         <v>2</v>
       </c>
     </row>
@@ -887,7 +892,7 @@
         <v>2.5</v>
       </c>
       <c r="E4" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>1.7</v>
       </c>
       <c r="F4" s="10">
@@ -895,57 +900,57 @@
         <v>5.4</v>
       </c>
       <c r="G4" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>2.5</v>
       </c>
       <c r="H4" s="9">
-        <f t="shared" si="0"/>
+        <f>G4+T4</f>
         <v>2.8</v>
       </c>
-      <c r="I4" s="9">
+      <c r="I4" s="1">
+        <f>H4-G4</f>
+        <v>0.29999999999999982</v>
+      </c>
+      <c r="J4" s="9">
         <v>2.89</v>
       </c>
-      <c r="J4" s="1">
-        <f t="shared" si="8"/>
+      <c r="K4" s="1">
+        <f>J4-G4</f>
         <v>0.39000000000000012</v>
       </c>
-      <c r="K4" s="1">
-        <f t="shared" si="1"/>
-        <v>0.29999999999999982</v>
-      </c>
       <c r="L4" s="4">
-        <f t="shared" si="2"/>
+        <f>I4/G4</f>
         <v>0.11999999999999993</v>
       </c>
       <c r="M4" s="8">
         <v>12</v>
       </c>
       <c r="N4" s="5">
+        <f t="shared" si="0"/>
+        <v>5.6338028169014086E-2</v>
+      </c>
+      <c r="O4" s="3">
         <f t="shared" si="3"/>
-        <v>5.6338028169014086E-2</v>
-      </c>
-      <c r="O4" s="3">
-        <f t="shared" si="9"/>
         <v>0.05</v>
       </c>
       <c r="P4" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="4"/>
         <v>6.338028169014083E-3</v>
       </c>
       <c r="Q4" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>9.5070422535211252E-2</v>
       </c>
       <c r="R4" s="1">
-        <f t="shared" si="4"/>
+        <f>G4-E4</f>
         <v>0.8</v>
       </c>
       <c r="S4" s="1">
-        <f t="shared" si="5"/>
+        <f>F4-D4</f>
         <v>2.9000000000000004</v>
       </c>
       <c r="T4" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>0.3</v>
       </c>
     </row>
@@ -963,7 +968,7 @@
         <v>3</v>
       </c>
       <c r="E5" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>1.9</v>
       </c>
       <c r="F5" s="10">
@@ -971,57 +976,57 @@
         <v>3.7</v>
       </c>
       <c r="G5" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="H5" s="9">
-        <f t="shared" si="0"/>
+        <f>G5+T5</f>
         <v>3.9</v>
       </c>
-      <c r="I5" s="9">
+      <c r="I5" s="1">
+        <f>H5-G5</f>
+        <v>0.89999999999999991</v>
+      </c>
+      <c r="J5" s="9">
         <v>3.58</v>
       </c>
-      <c r="J5" s="1">
-        <f t="shared" si="8"/>
+      <c r="K5" s="1">
+        <f>J5-G5</f>
         <v>0.58000000000000007</v>
       </c>
-      <c r="K5" s="1">
-        <f t="shared" si="1"/>
-        <v>0.89999999999999991</v>
-      </c>
       <c r="L5" s="4">
-        <f t="shared" si="2"/>
+        <f>I5/G5</f>
         <v>0.3</v>
       </c>
       <c r="M5" s="8">
         <v>28</v>
       </c>
       <c r="N5" s="5">
+        <f t="shared" si="0"/>
+        <v>0.13145539906103287</v>
+      </c>
+      <c r="O5" s="3">
         <f t="shared" si="3"/>
-        <v>0.13145539906103287</v>
-      </c>
-      <c r="O5" s="3">
-        <f t="shared" si="9"/>
         <v>0.05</v>
       </c>
       <c r="P5" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="4"/>
         <v>8.1455399061032871E-2</v>
       </c>
       <c r="Q5" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>1.221830985915493</v>
       </c>
       <c r="R5" s="1">
-        <f t="shared" si="4"/>
+        <f>G5-E5</f>
         <v>1.1000000000000001</v>
       </c>
       <c r="S5" s="1">
-        <f t="shared" si="5"/>
+        <f>F5-D5</f>
         <v>0.70000000000000018</v>
       </c>
       <c r="T5" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>0.9</v>
       </c>
     </row>
@@ -1039,65 +1044,65 @@
         <v>3</v>
       </c>
       <c r="E6" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>1.9</v>
       </c>
       <c r="F6" s="10">
-        <f t="shared" ref="F6:F19" si="13">ROUND(4*C6,1)</f>
+        <f t="shared" ref="F6:F19" si="7">ROUND(4*C6,1)</f>
         <v>5.4</v>
       </c>
       <c r="G6" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="H6" s="9">
-        <f t="shared" si="0"/>
+        <f>G6+T6</f>
         <v>3.2</v>
       </c>
-      <c r="I6" s="9">
+      <c r="I6" s="1">
+        <f>H6-G6</f>
+        <v>0.20000000000000018</v>
+      </c>
+      <c r="J6" s="9">
         <v>2.82</v>
       </c>
-      <c r="J6" s="1">
-        <f t="shared" si="8"/>
+      <c r="K6" s="1">
+        <f>J6-G6</f>
         <v>-0.18000000000000016</v>
       </c>
-      <c r="K6" s="1">
-        <f t="shared" si="1"/>
-        <v>0.20000000000000018</v>
-      </c>
       <c r="L6" s="4">
-        <f t="shared" si="2"/>
+        <f>I6/G6</f>
         <v>6.6666666666666721E-2</v>
       </c>
       <c r="M6" s="8">
         <v>12</v>
       </c>
       <c r="N6" s="5">
+        <f t="shared" si="0"/>
+        <v>5.6338028169014086E-2</v>
+      </c>
+      <c r="O6" s="3">
         <f t="shared" si="3"/>
-        <v>5.6338028169014086E-2</v>
-      </c>
-      <c r="O6" s="3">
-        <f t="shared" si="9"/>
         <v>0.05</v>
       </c>
       <c r="P6" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="4"/>
         <v>6.338028169014083E-3</v>
       </c>
       <c r="Q6" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>9.5070422535211252E-2</v>
       </c>
       <c r="R6" s="1">
-        <f t="shared" si="4"/>
+        <f>G6-E6</f>
         <v>1.1000000000000001</v>
       </c>
       <c r="S6" s="1">
-        <f t="shared" si="5"/>
+        <f>F6-D6</f>
         <v>2.4000000000000004</v>
       </c>
       <c r="T6" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>0.2</v>
       </c>
     </row>
@@ -1115,65 +1120,65 @@
         <v>4</v>
       </c>
       <c r="E7" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="F7" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="7"/>
         <v>5.9</v>
       </c>
       <c r="G7" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="H7" s="9">
-        <f t="shared" si="0"/>
+        <f>G7+T7</f>
         <v>2.8</v>
       </c>
-      <c r="I7" s="9">
+      <c r="I7" s="1">
+        <f>H7-G7</f>
+        <v>-1.2000000000000002</v>
+      </c>
+      <c r="J7" s="9">
         <v>2.66</v>
       </c>
-      <c r="J7" s="1">
-        <f t="shared" si="8"/>
+      <c r="K7" s="1">
+        <f>J7-G7</f>
         <v>-1.3399999999999999</v>
       </c>
-      <c r="K7" s="1">
-        <f t="shared" si="1"/>
-        <v>-1.2000000000000002</v>
-      </c>
       <c r="L7" s="4">
-        <f t="shared" si="2"/>
+        <f>I7/G7</f>
         <v>-0.30000000000000004</v>
       </c>
       <c r="M7" s="8">
         <v>2</v>
       </c>
       <c r="N7" s="5">
+        <f t="shared" si="0"/>
+        <v>9.3896713615023476E-3</v>
+      </c>
+      <c r="O7" s="3">
         <f t="shared" si="3"/>
-        <v>9.3896713615023476E-3</v>
-      </c>
-      <c r="O7" s="3">
-        <f t="shared" si="9"/>
         <v>0.05</v>
       </c>
       <c r="P7" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="4"/>
         <v>-4.0610328638497659E-2</v>
       </c>
       <c r="Q7" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>-0.60915492957746487</v>
       </c>
       <c r="R7" s="1">
-        <f t="shared" si="4"/>
+        <f>G7-E7</f>
         <v>2</v>
       </c>
       <c r="S7" s="1">
-        <f t="shared" si="5"/>
+        <f>F7-D7</f>
         <v>1.9000000000000004</v>
       </c>
       <c r="T7" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>-1.2</v>
       </c>
     </row>
@@ -1191,65 +1196,65 @@
         <v>4</v>
       </c>
       <c r="E8" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>2.4</v>
       </c>
       <c r="F8" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="7"/>
         <v>7.7</v>
       </c>
       <c r="G8" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="H8" s="9">
-        <f t="shared" si="0"/>
+        <f>G8+T8</f>
         <v>4.9000000000000004</v>
       </c>
-      <c r="I8" s="9">
+      <c r="I8" s="1">
+        <f>H8-G8</f>
+        <v>0.90000000000000036</v>
+      </c>
+      <c r="J8" s="9">
         <v>7.7</v>
       </c>
-      <c r="J8" s="1">
-        <f t="shared" si="8"/>
+      <c r="K8" s="1">
+        <f>J8-G8</f>
         <v>3.7</v>
       </c>
-      <c r="K8" s="1">
-        <f t="shared" si="1"/>
-        <v>0.90000000000000036</v>
-      </c>
       <c r="L8" s="4">
-        <f t="shared" si="2"/>
+        <f>I8/G8</f>
         <v>0.22500000000000009</v>
       </c>
       <c r="M8" s="8">
         <v>14</v>
       </c>
       <c r="N8" s="5">
+        <f t="shared" si="0"/>
+        <v>6.5727699530516437E-2</v>
+      </c>
+      <c r="O8" s="3">
         <f t="shared" si="3"/>
-        <v>6.5727699530516437E-2</v>
-      </c>
-      <c r="O8" s="3">
-        <f t="shared" si="9"/>
         <v>0.05</v>
       </c>
       <c r="P8" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="4"/>
         <v>1.5727699530516434E-2</v>
       </c>
       <c r="Q8" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>0.2359154929577465</v>
       </c>
       <c r="R8" s="1">
-        <f t="shared" si="4"/>
+        <f>G8-E8</f>
         <v>1.6</v>
       </c>
       <c r="S8" s="1">
-        <f t="shared" si="5"/>
+        <f>F8-D8</f>
         <v>3.7</v>
       </c>
       <c r="T8" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>0.9</v>
       </c>
     </row>
@@ -1267,65 +1272,65 @@
         <v>4</v>
       </c>
       <c r="E9" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>2.5</v>
       </c>
       <c r="F9" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
       <c r="G9" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="H9" s="9">
-        <f t="shared" si="0"/>
+        <f>G9+T9</f>
         <v>6.1</v>
       </c>
-      <c r="I9" s="9">
+      <c r="I9" s="1">
+        <f>H9-G9</f>
+        <v>2.0999999999999996</v>
+      </c>
+      <c r="J9" s="9">
         <v>4.68</v>
       </c>
-      <c r="J9" s="1">
-        <f t="shared" si="8"/>
+      <c r="K9" s="1">
+        <f>J9-G9</f>
         <v>0.67999999999999972</v>
       </c>
-      <c r="K9" s="1">
-        <f t="shared" si="1"/>
-        <v>2.0999999999999996</v>
-      </c>
       <c r="L9" s="4">
-        <f t="shared" si="2"/>
+        <f>I9/G9</f>
         <v>0.52499999999999991</v>
       </c>
       <c r="M9" s="8">
         <v>18</v>
       </c>
       <c r="N9" s="5">
+        <f t="shared" si="0"/>
+        <v>8.4507042253521125E-2</v>
+      </c>
+      <c r="O9" s="3">
         <f t="shared" si="3"/>
-        <v>8.4507042253521125E-2</v>
-      </c>
-      <c r="O9" s="3">
-        <f t="shared" si="9"/>
         <v>0.05</v>
       </c>
       <c r="P9" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="4"/>
         <v>3.4507042253521122E-2</v>
       </c>
       <c r="Q9" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>0.51760563380281688</v>
       </c>
       <c r="R9" s="1">
-        <f t="shared" si="4"/>
+        <f>G9-E9</f>
         <v>1.5</v>
       </c>
       <c r="S9" s="1">
-        <f t="shared" si="5"/>
+        <f>F9-D9</f>
         <v>4</v>
       </c>
       <c r="T9" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>2.1</v>
       </c>
     </row>
@@ -1343,65 +1348,65 @@
         <v>4</v>
       </c>
       <c r="E10" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>2.6</v>
       </c>
       <c r="F10" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="7"/>
         <v>8.4</v>
       </c>
       <c r="G10" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="H10" s="9">
-        <f t="shared" si="0"/>
+        <f>G10+T10</f>
         <v>4.7</v>
       </c>
-      <c r="I10" s="9">
+      <c r="I10" s="1">
+        <f>H10-G10</f>
+        <v>0.70000000000000018</v>
+      </c>
+      <c r="J10" s="9">
         <v>3.93</v>
       </c>
-      <c r="J10" s="1">
-        <f t="shared" si="8"/>
+      <c r="K10" s="1">
+        <f>J10-G10</f>
         <v>-6.999999999999984E-2</v>
       </c>
-      <c r="K10" s="1">
-        <f t="shared" si="1"/>
-        <v>0.70000000000000018</v>
-      </c>
       <c r="L10" s="4">
-        <f t="shared" si="2"/>
+        <f>I10/G10</f>
         <v>0.17500000000000004</v>
       </c>
       <c r="M10" s="8">
         <v>13</v>
       </c>
       <c r="N10" s="5">
+        <f t="shared" si="0"/>
+        <v>6.1032863849765258E-2</v>
+      </c>
+      <c r="O10" s="3">
         <f t="shared" si="3"/>
-        <v>6.1032863849765258E-2</v>
-      </c>
-      <c r="O10" s="3">
-        <f t="shared" si="9"/>
         <v>0.05</v>
       </c>
       <c r="P10" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="4"/>
         <v>1.1032863849765255E-2</v>
       </c>
       <c r="Q10" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>0.16549295774647882</v>
       </c>
       <c r="R10" s="1">
-        <f t="shared" si="4"/>
+        <f>G10-E10</f>
         <v>1.4</v>
       </c>
       <c r="S10" s="1">
-        <f t="shared" si="5"/>
+        <f>F10-D10</f>
         <v>4.4000000000000004</v>
       </c>
       <c r="T10" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>0.7</v>
       </c>
     </row>
@@ -1419,65 +1424,65 @@
         <v>4</v>
       </c>
       <c r="E11" s="10">
+        <f t="shared" si="1"/>
+        <v>1.9</v>
+      </c>
+      <c r="F11" s="10">
+        <f t="shared" si="7"/>
+        <v>5.8</v>
+      </c>
+      <c r="G11" s="1">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="H11" s="9">
+        <f>G11+T11</f>
+        <v>3</v>
+      </c>
+      <c r="I11" s="1">
+        <f>H11-G11</f>
+        <v>-1</v>
+      </c>
+      <c r="J11" s="9">
+        <v>2.66</v>
+      </c>
+      <c r="K11" s="1">
+        <f>J11-G11</f>
+        <v>-1.3399999999999999</v>
+      </c>
+      <c r="L11" s="4">
+        <f>I11/G11</f>
+        <v>-0.25</v>
+      </c>
+      <c r="M11" s="8">
+        <v>4</v>
+      </c>
+      <c r="N11" s="5">
+        <f t="shared" si="0"/>
+        <v>1.8779342723004695E-2</v>
+      </c>
+      <c r="O11" s="3">
+        <f t="shared" si="3"/>
+        <v>0.05</v>
+      </c>
+      <c r="P11" s="6">
+        <f t="shared" si="4"/>
+        <v>-3.1220657276995308E-2</v>
+      </c>
+      <c r="Q11" s="3">
+        <f t="shared" si="5"/>
+        <v>-0.46830985915492962</v>
+      </c>
+      <c r="R11" s="1">
+        <f>G11-E11</f>
+        <v>2.1</v>
+      </c>
+      <c r="S11" s="1">
+        <f>F11-D11</f>
+        <v>1.7999999999999998</v>
+      </c>
+      <c r="T11" s="2">
         <f t="shared" si="6"/>
-        <v>1.9</v>
-      </c>
-      <c r="F11" s="10">
-        <f t="shared" si="13"/>
-        <v>5.8</v>
-      </c>
-      <c r="G11" s="1">
-        <f t="shared" si="7"/>
-        <v>4</v>
-      </c>
-      <c r="H11" s="9">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="I11" s="9">
-        <v>2.66</v>
-      </c>
-      <c r="J11" s="1">
-        <f t="shared" si="8"/>
-        <v>-1.3399999999999999</v>
-      </c>
-      <c r="K11" s="1">
-        <f t="shared" si="1"/>
-        <v>-1</v>
-      </c>
-      <c r="L11" s="4">
-        <f t="shared" si="2"/>
-        <v>-0.25</v>
-      </c>
-      <c r="M11" s="8">
-        <v>4</v>
-      </c>
-      <c r="N11" s="5">
-        <f t="shared" si="3"/>
-        <v>1.8779342723004695E-2</v>
-      </c>
-      <c r="O11" s="3">
-        <f t="shared" si="9"/>
-        <v>0.05</v>
-      </c>
-      <c r="P11" s="6">
-        <f t="shared" si="10"/>
-        <v>-3.1220657276995308E-2</v>
-      </c>
-      <c r="Q11" s="3">
-        <f t="shared" si="11"/>
-        <v>-0.46830985915492962</v>
-      </c>
-      <c r="R11" s="1">
-        <f t="shared" si="4"/>
-        <v>2.1</v>
-      </c>
-      <c r="S11" s="1">
-        <f t="shared" si="5"/>
-        <v>1.7999999999999998</v>
-      </c>
-      <c r="T11" s="2">
-        <f t="shared" si="12"/>
         <v>-1</v>
       </c>
     </row>
@@ -1495,65 +1500,65 @@
         <v>4</v>
       </c>
       <c r="E12" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>2.1</v>
       </c>
       <c r="F12" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="7"/>
         <v>6.5</v>
       </c>
       <c r="G12" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="H12" s="9">
-        <f t="shared" si="0"/>
+        <f>G12+T12</f>
         <v>3</v>
       </c>
-      <c r="I12" s="9">
+      <c r="I12" s="1">
+        <f>H12-G12</f>
+        <v>-1</v>
+      </c>
+      <c r="J12" s="9">
         <v>3.29</v>
       </c>
-      <c r="J12" s="1">
-        <f t="shared" si="8"/>
+      <c r="K12" s="1">
+        <f>J12-G12</f>
         <v>-0.71</v>
       </c>
-      <c r="K12" s="1">
-        <f t="shared" si="1"/>
-        <v>-1</v>
-      </c>
       <c r="L12" s="4">
-        <f t="shared" si="2"/>
+        <f>I12/G12</f>
         <v>-0.25</v>
       </c>
       <c r="M12" s="8">
         <v>3</v>
       </c>
       <c r="N12" s="5">
+        <f t="shared" si="0"/>
+        <v>1.4084507042253521E-2</v>
+      </c>
+      <c r="O12" s="3">
         <f t="shared" si="3"/>
-        <v>1.4084507042253521E-2</v>
-      </c>
-      <c r="O12" s="3">
-        <f t="shared" si="9"/>
         <v>0.05</v>
       </c>
       <c r="P12" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="4"/>
         <v>-3.591549295774648E-2</v>
       </c>
       <c r="Q12" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>-0.53873239436619724</v>
       </c>
       <c r="R12" s="1">
-        <f t="shared" si="4"/>
+        <f>G12-E12</f>
         <v>1.9</v>
       </c>
       <c r="S12" s="1">
-        <f t="shared" si="5"/>
+        <f>F12-D12</f>
         <v>2.5</v>
       </c>
       <c r="T12" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>-1</v>
       </c>
     </row>
@@ -1571,65 +1576,65 @@
         <v>3</v>
       </c>
       <c r="E13" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>1.9</v>
       </c>
       <c r="F13" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="7"/>
         <v>5.7</v>
       </c>
       <c r="G13" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="H13" s="9">
-        <f t="shared" si="0"/>
+        <f>G13+T13</f>
         <v>2.8</v>
       </c>
-      <c r="I13" s="9">
+      <c r="I13" s="1">
+        <f>H13-G13</f>
+        <v>-0.20000000000000018</v>
+      </c>
+      <c r="J13" s="9">
         <v>3.49</v>
       </c>
-      <c r="J13" s="1">
-        <f t="shared" si="8"/>
+      <c r="K13" s="1">
+        <f>J13-G13</f>
         <v>0.49000000000000021</v>
       </c>
-      <c r="K13" s="1">
-        <f t="shared" si="1"/>
-        <v>-0.20000000000000018</v>
-      </c>
       <c r="L13" s="4">
-        <f t="shared" si="2"/>
+        <f>I13/G13</f>
         <v>-6.6666666666666721E-2</v>
       </c>
       <c r="M13" s="8">
         <v>8</v>
       </c>
       <c r="N13" s="5">
+        <f t="shared" si="0"/>
+        <v>3.7558685446009391E-2</v>
+      </c>
+      <c r="O13" s="3">
         <f t="shared" si="3"/>
-        <v>3.7558685446009391E-2</v>
-      </c>
-      <c r="O13" s="3">
-        <f t="shared" si="9"/>
         <v>0.05</v>
       </c>
       <c r="P13" s="6">
-        <f t="shared" ref="P13:P19" si="14">N13-O13</f>
+        <f t="shared" ref="P13:P19" si="8">N13-O13</f>
         <v>-1.2441314553990612E-2</v>
       </c>
       <c r="Q13" s="3">
-        <f t="shared" ref="Q13:Q19" si="15">P13*$U$2</f>
+        <f t="shared" ref="Q13:Q19" si="9">P13*$U$2</f>
         <v>-0.18661971830985918</v>
       </c>
       <c r="R13" s="1">
-        <f t="shared" si="4"/>
+        <f>G13-E13</f>
         <v>1.1000000000000001</v>
       </c>
       <c r="S13" s="1">
-        <f t="shared" si="5"/>
+        <f>F13-D13</f>
         <v>2.7</v>
       </c>
       <c r="T13" s="2">
-        <f t="shared" ref="T13:T19" si="16">ROUND(IF(P13&gt;0,S13*Q13,R13*Q13),1)</f>
+        <f t="shared" ref="T13:T19" si="10">ROUND(IF(P13&gt;0,S13*Q13,R13*Q13),1)</f>
         <v>-0.2</v>
       </c>
     </row>
@@ -1648,65 +1653,65 @@
         <v>4</v>
       </c>
       <c r="E14" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>1.8</v>
       </c>
       <c r="F14" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="7"/>
         <v>5.4</v>
       </c>
       <c r="G14" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="H14" s="9">
-        <f t="shared" si="0"/>
+        <f>G14+T14</f>
         <v>3.9</v>
       </c>
-      <c r="I14" s="9">
+      <c r="I14" s="1">
+        <f>H14-G14</f>
+        <v>-0.10000000000000009</v>
+      </c>
+      <c r="J14" s="9">
         <v>2.0099999999999998</v>
       </c>
-      <c r="J14" s="1">
-        <f t="shared" si="8"/>
+      <c r="K14" s="1">
+        <f>J14-G14</f>
         <v>-1.9900000000000002</v>
       </c>
-      <c r="K14" s="1">
-        <f t="shared" si="1"/>
-        <v>-0.10000000000000009</v>
-      </c>
       <c r="L14" s="4">
-        <f t="shared" si="2"/>
+        <f>I14/G14</f>
         <v>-2.5000000000000022E-2</v>
       </c>
       <c r="M14" s="8">
         <v>10</v>
       </c>
       <c r="N14" s="5">
+        <f t="shared" si="0"/>
+        <v>4.6948356807511735E-2</v>
+      </c>
+      <c r="O14" s="3">
         <f t="shared" si="3"/>
-        <v>4.6948356807511735E-2</v>
-      </c>
-      <c r="O14" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="P14" s="6">
+        <f t="shared" si="8"/>
+        <v>-3.0516431924882681E-3</v>
+      </c>
+      <c r="Q14" s="3">
         <f t="shared" si="9"/>
-        <v>0.05</v>
-      </c>
-      <c r="P14" s="6">
-        <f t="shared" si="14"/>
-        <v>-3.0516431924882681E-3</v>
-      </c>
-      <c r="Q14" s="3">
-        <f t="shared" si="15"/>
         <v>-4.5774647887324021E-2</v>
       </c>
       <c r="R14" s="1">
-        <f t="shared" si="4"/>
+        <f>G14-E14</f>
         <v>2.2000000000000002</v>
       </c>
       <c r="S14" s="1">
-        <f t="shared" si="5"/>
+        <f>F14-D14</f>
         <v>1.4000000000000004</v>
       </c>
       <c r="T14" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>-0.1</v>
       </c>
     </row>
@@ -1724,65 +1729,65 @@
         <v>4</v>
       </c>
       <c r="E15" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>2.2999999999999998</v>
       </c>
       <c r="F15" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="7"/>
         <v>7.4</v>
       </c>
       <c r="G15" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="H15" s="9">
-        <f t="shared" si="0"/>
+        <f>G15+T15</f>
         <v>6.2</v>
       </c>
-      <c r="I15" s="9">
+      <c r="I15" s="1">
+        <f>H15-G15</f>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="J15" s="9">
         <v>6.36</v>
       </c>
-      <c r="J15" s="1">
-        <f t="shared" si="8"/>
+      <c r="K15" s="1">
+        <f>J15-G15</f>
         <v>2.3600000000000003</v>
       </c>
-      <c r="K15" s="1">
-        <f t="shared" si="1"/>
-        <v>2.2000000000000002</v>
-      </c>
       <c r="L15" s="4">
-        <f t="shared" si="2"/>
+        <f>I15/G15</f>
         <v>0.55000000000000004</v>
       </c>
       <c r="M15" s="8">
         <v>20</v>
       </c>
       <c r="N15" s="5">
+        <f t="shared" si="0"/>
+        <v>9.3896713615023469E-2</v>
+      </c>
+      <c r="O15" s="3">
         <f t="shared" si="3"/>
-        <v>9.3896713615023469E-2</v>
-      </c>
-      <c r="O15" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="P15" s="6">
+        <f t="shared" si="8"/>
+        <v>4.3896713615023467E-2</v>
+      </c>
+      <c r="Q15" s="3">
         <f t="shared" si="9"/>
-        <v>0.05</v>
-      </c>
-      <c r="P15" s="6">
-        <f t="shared" si="14"/>
-        <v>4.3896713615023467E-2</v>
-      </c>
-      <c r="Q15" s="3">
-        <f t="shared" si="15"/>
         <v>0.65845070422535201</v>
       </c>
       <c r="R15" s="1">
-        <f t="shared" si="4"/>
+        <f>G15-E15</f>
         <v>1.7000000000000002</v>
       </c>
       <c r="S15" s="1">
-        <f t="shared" si="5"/>
+        <f>F15-D15</f>
         <v>3.4000000000000004</v>
       </c>
       <c r="T15" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>2.2000000000000002</v>
       </c>
     </row>
@@ -1800,65 +1805,65 @@
         <v>4</v>
       </c>
       <c r="E16" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>2.5</v>
       </c>
       <c r="F16" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="7"/>
         <v>7.9</v>
       </c>
       <c r="G16" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="H16" s="9">
-        <f t="shared" si="0"/>
+        <f>G16+T16</f>
         <v>3.9</v>
       </c>
-      <c r="I16" s="9">
+      <c r="I16" s="1">
+        <f>H16-G16</f>
+        <v>-0.10000000000000009</v>
+      </c>
+      <c r="J16" s="9">
         <v>5.59</v>
       </c>
-      <c r="J16" s="1">
-        <f t="shared" si="8"/>
+      <c r="K16" s="1">
+        <f>J16-G16</f>
         <v>1.5899999999999999</v>
       </c>
-      <c r="K16" s="1">
-        <f t="shared" si="1"/>
-        <v>-0.10000000000000009</v>
-      </c>
       <c r="L16" s="4">
-        <f t="shared" si="2"/>
+        <f>I16/G16</f>
         <v>-2.5000000000000022E-2</v>
       </c>
       <c r="M16" s="8">
         <v>10</v>
       </c>
       <c r="N16" s="5">
+        <f t="shared" si="0"/>
+        <v>4.6948356807511735E-2</v>
+      </c>
+      <c r="O16" s="3">
         <f t="shared" si="3"/>
-        <v>4.6948356807511735E-2</v>
-      </c>
-      <c r="O16" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="P16" s="6">
+        <f t="shared" si="8"/>
+        <v>-3.0516431924882681E-3</v>
+      </c>
+      <c r="Q16" s="3">
         <f t="shared" si="9"/>
-        <v>0.05</v>
-      </c>
-      <c r="P16" s="6">
-        <f t="shared" si="14"/>
-        <v>-3.0516431924882681E-3</v>
-      </c>
-      <c r="Q16" s="3">
-        <f t="shared" si="15"/>
         <v>-4.5774647887324021E-2</v>
       </c>
       <c r="R16" s="1">
-        <f t="shared" si="4"/>
+        <f>G16-E16</f>
         <v>1.5</v>
       </c>
       <c r="S16" s="1">
-        <f t="shared" si="5"/>
+        <f>F16-D16</f>
         <v>3.9000000000000004</v>
       </c>
       <c r="T16" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>-0.1</v>
       </c>
     </row>
@@ -1876,41 +1881,41 @@
         <v>4</v>
       </c>
       <c r="E17" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>2.8</v>
       </c>
       <c r="F17" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="7"/>
         <v>9.1999999999999993</v>
       </c>
       <c r="G17" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="H17" s="9">
+        <f>G17+T17</f>
+        <v>3.4</v>
+      </c>
+      <c r="I17" s="1">
+        <f>H17-G17</f>
+        <v>-0.60000000000000009</v>
+      </c>
+      <c r="J17" s="9">
+        <v>4.87</v>
+      </c>
+      <c r="K17" s="1">
+        <f>J17-G17</f>
+        <v>0.87000000000000011</v>
+      </c>
+      <c r="L17" s="4">
+        <f>I17/G17</f>
+        <v>-0.15000000000000002</v>
+      </c>
+      <c r="M17" s="8">
+        <v>4</v>
+      </c>
+      <c r="N17" s="5">
         <f t="shared" si="0"/>
-        <v>3.4</v>
-      </c>
-      <c r="I17" s="9">
-        <v>4.87</v>
-      </c>
-      <c r="J17" s="1">
-        <f t="shared" si="8"/>
-        <v>0.87000000000000011</v>
-      </c>
-      <c r="K17" s="1">
-        <f t="shared" si="1"/>
-        <v>-0.60000000000000009</v>
-      </c>
-      <c r="L17" s="4">
-        <f t="shared" si="2"/>
-        <v>-0.15000000000000002</v>
-      </c>
-      <c r="M17" s="8">
-        <v>4</v>
-      </c>
-      <c r="N17" s="5">
-        <f t="shared" si="3"/>
         <v>1.8779342723004695E-2</v>
       </c>
       <c r="O17" s="3">
@@ -1918,23 +1923,23 @@
         <v>0.05</v>
       </c>
       <c r="P17" s="6">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v>-3.1220657276995308E-2</v>
       </c>
       <c r="Q17" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>-0.46830985915492962</v>
       </c>
       <c r="R17" s="1">
-        <f t="shared" si="4"/>
+        <f>G17-E17</f>
         <v>1.2000000000000002</v>
       </c>
       <c r="S17" s="1">
-        <f t="shared" si="5"/>
+        <f>F17-D17</f>
         <v>5.1999999999999993</v>
       </c>
       <c r="T17" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>-0.6</v>
       </c>
     </row>
@@ -1952,65 +1957,65 @@
         <v>4</v>
       </c>
       <c r="E18" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>2.4</v>
       </c>
       <c r="F18" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="7"/>
         <v>7.6</v>
       </c>
       <c r="G18" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="H18" s="9">
-        <f t="shared" si="0"/>
+        <f>G18+T18</f>
         <v>5.9</v>
       </c>
-      <c r="I18" s="9">
+      <c r="I18" s="1">
+        <f>H18-G18</f>
+        <v>1.9000000000000004</v>
+      </c>
+      <c r="J18" s="9">
         <v>3.17</v>
       </c>
-      <c r="J18" s="1">
-        <f t="shared" si="8"/>
+      <c r="K18" s="1">
+        <f>J18-G18</f>
         <v>-0.83000000000000007</v>
       </c>
-      <c r="K18" s="1">
-        <f t="shared" si="1"/>
-        <v>1.9000000000000004</v>
-      </c>
       <c r="L18" s="4">
-        <f t="shared" si="2"/>
+        <f>I18/G18</f>
         <v>0.47500000000000009</v>
       </c>
       <c r="M18" s="8">
         <v>18</v>
       </c>
       <c r="N18" s="5">
+        <f t="shared" si="0"/>
+        <v>8.4507042253521125E-2</v>
+      </c>
+      <c r="O18" s="3">
         <f t="shared" si="3"/>
-        <v>8.4507042253521125E-2</v>
-      </c>
-      <c r="O18" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="P18" s="6">
+        <f t="shared" si="8"/>
+        <v>3.4507042253521122E-2</v>
+      </c>
+      <c r="Q18" s="3">
         <f t="shared" si="9"/>
-        <v>0.05</v>
-      </c>
-      <c r="P18" s="6">
-        <f t="shared" si="14"/>
-        <v>3.4507042253521122E-2</v>
-      </c>
-      <c r="Q18" s="3">
-        <f t="shared" si="15"/>
         <v>0.51760563380281688</v>
       </c>
       <c r="R18" s="1">
-        <f t="shared" si="4"/>
+        <f>G18-E18</f>
         <v>1.6</v>
       </c>
       <c r="S18" s="1">
-        <f t="shared" si="5"/>
+        <f>F18-D18</f>
         <v>3.5999999999999996</v>
       </c>
       <c r="T18" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>1.9</v>
       </c>
     </row>
@@ -2022,72 +2027,72 @@
         <v>44</v>
       </c>
       <c r="C19" s="2">
-        <v>2.2999999999999998</v>
+        <v>1.98</v>
       </c>
       <c r="D19" s="10">
         <v>4</v>
       </c>
       <c r="E19" s="10">
-        <f t="shared" si="6"/>
-        <v>2.8</v>
+        <f t="shared" si="1"/>
+        <v>2.5</v>
       </c>
       <c r="F19" s="10">
-        <f t="shared" si="13"/>
-        <v>9.1999999999999993</v>
+        <f t="shared" si="7"/>
+        <v>7.9</v>
       </c>
       <c r="G19" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="H19" s="9">
-        <f t="shared" si="0"/>
-        <v>5.6</v>
-      </c>
-      <c r="I19" s="9">
+        <f>G19+T19</f>
+        <v>5.2</v>
+      </c>
+      <c r="I19" s="1">
+        <f>H19-G19</f>
+        <v>1.2000000000000002</v>
+      </c>
+      <c r="J19" s="9">
         <v>5.65</v>
       </c>
-      <c r="J19" s="1">
-        <f t="shared" si="8"/>
+      <c r="K19" s="1">
+        <f>J19-G19</f>
         <v>1.6500000000000004</v>
       </c>
-      <c r="K19" s="1">
-        <f t="shared" si="1"/>
-        <v>1.5999999999999996</v>
-      </c>
       <c r="L19" s="4">
-        <f t="shared" si="2"/>
-        <v>0.39999999999999991</v>
+        <f>I19/G19</f>
+        <v>0.30000000000000004</v>
       </c>
       <c r="M19" s="8">
         <v>15</v>
       </c>
       <c r="N19" s="5">
+        <f t="shared" si="0"/>
+        <v>7.0422535211267609E-2</v>
+      </c>
+      <c r="O19" s="3">
         <f t="shared" si="3"/>
-        <v>7.0422535211267609E-2</v>
-      </c>
-      <c r="O19" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="P19" s="6">
+        <f t="shared" si="8"/>
+        <v>2.0422535211267606E-2</v>
+      </c>
+      <c r="Q19" s="3">
         <f t="shared" si="9"/>
-        <v>0.05</v>
-      </c>
-      <c r="P19" s="6">
-        <f t="shared" si="14"/>
-        <v>2.0422535211267606E-2</v>
-      </c>
-      <c r="Q19" s="3">
-        <f t="shared" si="15"/>
         <v>0.30633802816901412</v>
       </c>
       <c r="R19" s="1">
-        <f t="shared" si="4"/>
-        <v>1.2000000000000002</v>
+        <f>G19-E19</f>
+        <v>1.5</v>
       </c>
       <c r="S19" s="1">
-        <f t="shared" si="5"/>
-        <v>5.1999999999999993</v>
+        <f>F19-D19</f>
+        <v>3.9000000000000004</v>
       </c>
       <c r="T19" s="2">
-        <f t="shared" si="16"/>
-        <v>1.6</v>
+        <f t="shared" si="10"/>
+        <v>1.2</v>
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
@@ -2171,7 +2176,7 @@
       <c r="B74"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="J2:L19">
+  <conditionalFormatting sqref="K2:L19 I2:I19">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>